<commit_message>
UI Enhancement: Redesign student list with avatars, better layout and visual hierarchy
</commit_message>
<xml_diff>
--- a/students_import.xlsx
+++ b/students_import.xlsx
@@ -397,104 +397,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>שם</v>
+        <v>שם פרטי</v>
+      </c>
+      <c r="B1" t="str">
+        <v>שם משפחה</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>אדרי ריף</v>
+        <v>ריף</v>
+      </c>
+      <c r="B2" t="str">
+        <v>אדרי</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>בנדרסקי ליאור</v>
+        <v>ליאור</v>
+      </c>
+      <c r="B3" t="str">
+        <v>בנדרסקי</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>גרובר בניה חיים</v>
+        <v>בניה חיים</v>
+      </c>
+      <c r="B4" t="str">
+        <v>גרובר</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>הנדורגר יותם</v>
+        <v>יותם</v>
+      </c>
+      <c r="B5" t="str">
+        <v>הנדורגר</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>זפרני יהלי</v>
+        <v>יהלי</v>
+      </c>
+      <c r="B6" t="str">
+        <v>זפרני</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>טיומקין עדן</v>
+        <v>עדן</v>
+      </c>
+      <c r="B7" t="str">
+        <v>טיומקין</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>טייב הראל אנריקה</v>
+        <v>הראל אנריקה</v>
+      </c>
+      <c r="B8" t="str">
+        <v>טייב</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>ילין לנדסקרו יוני</v>
+        <v>יוני</v>
+      </c>
+      <c r="B9" t="str">
+        <v>ילין לנדסקרו</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>ישראל מאיה</v>
+        <v>מאיה</v>
+      </c>
+      <c r="B10" t="str">
+        <v>ישראל</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>כחלון אורי דוד</v>
+        <v>אורי דוד</v>
+      </c>
+      <c r="B11" t="str">
+        <v>כחלון</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>לנדמן דור</v>
+        <v>דור</v>
+      </c>
+      <c r="B12" t="str">
+        <v>לנדמן</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>סלע מאי</v>
+        <v>מאי</v>
+      </c>
+      <c r="B13" t="str">
+        <v>סלע</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>פסטמן הראל</v>
+        <v>הראל</v>
+      </c>
+      <c r="B14" t="str">
+        <v>פסטמן</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>רובין עמית</v>
+        <v>עמית</v>
+      </c>
+      <c r="B15" t="str">
+        <v>רובין</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>שוסטרמן דנאל</v>
+        <v>דנאל</v>
+      </c>
+      <c r="B16" t="str">
+        <v>שוסטרמן</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>שיינברג יונתן</v>
+        <v>יונתן</v>
+      </c>
+      <c r="B17" t="str">
+        <v>שיינברג</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>שטופמכר עמית</v>
+        <v>עמית</v>
+      </c>
+      <c r="B18" t="str">
+        <v>שטופמכר</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>